<commit_message>
Small changes to Database setup
</commit_message>
<xml_diff>
--- a/src/main/resources/database_sample.xlsx
+++ b/src/main/resources/database_sample.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Noel\IdeaProjects\BikeRevolution\src\main\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CC7F4A43-4D34-4131-870D-8A26186FF478}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{368C0D73-7DD8-4EE6-BCD3-05D00D1BEB34}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{9068C110-C1AA-4A37-A3C4-5020E67D4199}"/>
+    <workbookView xWindow="22932" yWindow="1392" windowWidth="23256" windowHeight="12576" xr2:uid="{9068C110-C1AA-4A37-A3C4-5020E67D4199}"/>
   </bookViews>
   <sheets>
     <sheet name="Munka1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="64">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="71">
   <si>
     <t>Description</t>
   </si>
@@ -59,9 +59,6 @@
     <t>Hajtómű</t>
   </si>
   <si>
-    <t>Váltókábel</t>
-  </si>
-  <si>
     <t>Kormányfej</t>
   </si>
   <si>
@@ -83,9 +80,6 @@
     <t>Új lánc felszerelése</t>
   </si>
   <si>
-    <t>Fékállítás</t>
-  </si>
-  <si>
     <t>Fékalkatrészek beállítása vagy cseréje</t>
   </si>
   <si>
@@ -197,9 +191,6 @@
     <t>Fék bovden</t>
   </si>
   <si>
-    <t>PartCost</t>
-  </si>
-  <si>
     <t>ALL</t>
   </si>
   <si>
@@ -228,6 +219,36 @@
   </si>
   <si>
     <t>-1 lánc</t>
+  </si>
+  <si>
+    <t>Első hátsó külső gumi csere</t>
+  </si>
+  <si>
+    <t>Gumi Csere</t>
+  </si>
+  <si>
+    <t>-2 kulso gumi</t>
+  </si>
+  <si>
+    <t>ez nem kell</t>
+  </si>
+  <si>
+    <t>-2 pedal</t>
+  </si>
+  <si>
+    <t>-1 nyereg</t>
+  </si>
+  <si>
+    <t>Ez sem kell a táblába</t>
+  </si>
+  <si>
+    <t>Fékbetét Csere</t>
+  </si>
+  <si>
+    <t>-2 fekbetet</t>
+  </si>
+  <si>
+    <t>Váltó</t>
   </si>
 </sst>
 </file>
@@ -587,58 +608,58 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6EC0C065-1181-41F5-9F90-6272D8EE9D84}">
   <dimension ref="C1:O67"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D5" zoomScale="109" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="I10" sqref="I10"/>
+    <sheetView tabSelected="1" topLeftCell="D6" zoomScale="109" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="F13" sqref="F13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="2" width="8.88671875" style="1"/>
-    <col min="3" max="3" width="21.21875" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="34.6640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="11.33203125" style="1" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="17.88671875" style="1" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="29.77734375" style="1" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="34.88671875" style="1" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="14.6640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="1" max="2" width="8.85546875" style="1"/>
+    <col min="3" max="3" width="21.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="34.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="17.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="29.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="34.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="14.7109375" style="1" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="12" style="1" bestFit="1" customWidth="1"/>
-    <col min="11" max="12" width="8.88671875" style="1"/>
-    <col min="13" max="13" width="14.88671875" style="1" bestFit="1" customWidth="1"/>
-    <col min="14" max="16384" width="8.88671875" style="1"/>
+    <col min="11" max="12" width="8.85546875" style="1"/>
+    <col min="13" max="13" width="19.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="14" max="16384" width="8.85546875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="3:15" x14ac:dyDescent="0.3">
+    <row r="1" spans="3:15" x14ac:dyDescent="0.25">
       <c r="C1" s="1" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="4" spans="3:15" x14ac:dyDescent="0.3">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="4" spans="3:15" x14ac:dyDescent="0.25">
       <c r="D4" s="1" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="5" spans="3:15" x14ac:dyDescent="0.3">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="5" spans="3:15" x14ac:dyDescent="0.25">
       <c r="E5" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="F5" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="F5" s="1" t="s">
+      <c r="G5" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="G5" s="1" t="s">
-        <v>12</v>
-      </c>
       <c r="H5" s="1" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="O5"/>
     </row>
-    <row r="6" spans="3:15" x14ac:dyDescent="0.3">
+    <row r="6" spans="3:15" x14ac:dyDescent="0.25">
       <c r="E6" s="1">
         <v>1</v>
       </c>
@@ -653,12 +674,12 @@
       </c>
       <c r="O6"/>
     </row>
-    <row r="7" spans="3:15" x14ac:dyDescent="0.3">
+    <row r="7" spans="3:15" x14ac:dyDescent="0.25">
       <c r="E7" s="1">
         <v>2</v>
       </c>
       <c r="F7" s="1" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="G7" s="1">
         <v>50</v>
@@ -668,7 +689,7 @@
       </c>
       <c r="O7"/>
     </row>
-    <row r="8" spans="3:15" x14ac:dyDescent="0.3">
+    <row r="8" spans="3:15" x14ac:dyDescent="0.25">
       <c r="E8" s="1">
         <v>3</v>
       </c>
@@ -683,7 +704,7 @@
       </c>
       <c r="O8"/>
     </row>
-    <row r="9" spans="3:15" x14ac:dyDescent="0.3">
+    <row r="9" spans="3:15" x14ac:dyDescent="0.25">
       <c r="E9" s="1">
         <v>4</v>
       </c>
@@ -698,7 +719,7 @@
       </c>
       <c r="O9"/>
     </row>
-    <row r="10" spans="3:15" x14ac:dyDescent="0.3">
+    <row r="10" spans="3:15" x14ac:dyDescent="0.25">
       <c r="E10" s="1">
         <v>5</v>
       </c>
@@ -713,12 +734,12 @@
       </c>
       <c r="O10"/>
     </row>
-    <row r="11" spans="3:15" x14ac:dyDescent="0.3">
+    <row r="11" spans="3:15" x14ac:dyDescent="0.25">
       <c r="E11" s="1">
         <v>6</v>
       </c>
       <c r="F11" s="1" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="G11" s="1">
         <v>50</v>
@@ -728,7 +749,7 @@
       </c>
       <c r="O11"/>
     </row>
-    <row r="12" spans="3:15" x14ac:dyDescent="0.3">
+    <row r="12" spans="3:15" x14ac:dyDescent="0.25">
       <c r="E12" s="1">
         <v>7</v>
       </c>
@@ -743,33 +764,27 @@
       </c>
       <c r="O12"/>
     </row>
-    <row r="13" spans="3:15" x14ac:dyDescent="0.3">
+    <row r="13" spans="3:15" x14ac:dyDescent="0.25">
       <c r="E13" s="1">
         <v>8</v>
       </c>
       <c r="F13" s="1" t="s">
-        <v>7</v>
+        <v>70</v>
       </c>
       <c r="G13" s="1">
-        <v>35</v>
+        <v>20</v>
       </c>
       <c r="H13" s="1">
-        <v>12</v>
-      </c>
-      <c r="J13" s="1" t="s">
-        <v>53</v>
-      </c>
-      <c r="K13" s="1" t="s">
-        <v>54</v>
+        <v>20</v>
       </c>
       <c r="O13"/>
     </row>
-    <row r="14" spans="3:15" x14ac:dyDescent="0.3">
+    <row r="14" spans="3:15" x14ac:dyDescent="0.25">
       <c r="E14" s="1">
         <v>9</v>
       </c>
       <c r="F14" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="G14" s="1">
         <v>18</v>
@@ -779,27 +794,27 @@
       </c>
       <c r="O14"/>
     </row>
-    <row r="15" spans="3:15" x14ac:dyDescent="0.3">
+    <row r="15" spans="3:15" x14ac:dyDescent="0.25">
       <c r="E15" s="1">
         <v>10</v>
       </c>
       <c r="F15" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="G15" s="1">
         <v>30</v>
       </c>
       <c r="H15" s="1">
-        <v>15</v>
+        <v>5</v>
       </c>
       <c r="O15"/>
     </row>
-    <row r="16" spans="3:15" x14ac:dyDescent="0.3">
+    <row r="16" spans="3:15" x14ac:dyDescent="0.25">
       <c r="E16" s="1">
         <v>11</v>
       </c>
       <c r="F16" s="1" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="G16" s="1">
         <v>20</v>
@@ -809,12 +824,12 @@
       </c>
       <c r="O16"/>
     </row>
-    <row r="17" spans="4:15" x14ac:dyDescent="0.3">
+    <row r="17" spans="4:15" x14ac:dyDescent="0.25">
       <c r="E17" s="1">
         <v>12</v>
       </c>
       <c r="F17" s="1" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="G17" s="1">
         <v>20</v>
@@ -824,12 +839,12 @@
       </c>
       <c r="O17"/>
     </row>
-    <row r="18" spans="4:15" x14ac:dyDescent="0.3">
+    <row r="18" spans="4:15" x14ac:dyDescent="0.25">
       <c r="E18" s="1">
         <v>13</v>
       </c>
       <c r="F18" s="1" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="G18" s="1">
         <v>20</v>
@@ -839,12 +854,12 @@
       </c>
       <c r="O18"/>
     </row>
-    <row r="19" spans="4:15" x14ac:dyDescent="0.3">
+    <row r="19" spans="4:15" x14ac:dyDescent="0.25">
       <c r="E19" s="1">
         <v>14</v>
       </c>
       <c r="F19" s="1" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="G19" s="1">
         <v>15</v>
@@ -853,12 +868,12 @@
         <v>10</v>
       </c>
     </row>
-    <row r="20" spans="4:15" x14ac:dyDescent="0.3">
+    <row r="20" spans="4:15" x14ac:dyDescent="0.25">
       <c r="E20" s="1">
         <v>15</v>
       </c>
       <c r="F20" s="1" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="G20" s="1">
         <v>30</v>
@@ -867,46 +882,55 @@
         <v>5</v>
       </c>
     </row>
-    <row r="27" spans="4:15" x14ac:dyDescent="0.3">
+    <row r="27" spans="4:15" x14ac:dyDescent="0.25">
       <c r="D27" s="1" t="s">
         <v>1</v>
       </c>
       <c r="F27" s="1" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="28" spans="4:15" x14ac:dyDescent="0.3">
+        <v>32</v>
+      </c>
+      <c r="I27" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="J27" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="M27" s="1" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="28" spans="4:15" x14ac:dyDescent="0.25">
       <c r="F28" s="1" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="G28" s="1" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="H28" s="1" t="s">
         <v>0</v>
       </c>
       <c r="I28" s="1" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="J28" s="1" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="K28" s="1" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="M28" s="1" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="29" spans="4:15" x14ac:dyDescent="0.3">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="29" spans="4:15" x14ac:dyDescent="0.25">
       <c r="F29" s="1">
         <v>101</v>
       </c>
       <c r="G29" s="1" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="H29" s="1" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="I29" s="1">
         <v>15</v>
@@ -918,18 +942,18 @@
         <v>25</v>
       </c>
       <c r="M29" s="2" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="30" spans="4:15" x14ac:dyDescent="0.3">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="30" spans="4:15" x14ac:dyDescent="0.25">
       <c r="F30" s="1">
         <v>102</v>
       </c>
       <c r="G30" s="1" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="H30" s="1" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="I30" s="1">
         <v>10</v>
@@ -941,18 +965,18 @@
         <v>15</v>
       </c>
       <c r="M30" s="2" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="31" spans="4:15" x14ac:dyDescent="0.3">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="31" spans="4:15" x14ac:dyDescent="0.25">
       <c r="F31" s="1">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="G31" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="H31" s="1" t="s">
         <v>13</v>
-      </c>
-      <c r="H31" s="1" t="s">
-        <v>14</v>
       </c>
       <c r="I31" s="1">
         <v>20</v>
@@ -964,144 +988,194 @@
         <v>35</v>
       </c>
       <c r="M31" s="2" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="32" spans="4:15" x14ac:dyDescent="0.3">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="32" spans="4:15" x14ac:dyDescent="0.25">
       <c r="F32" s="1">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="G32" s="1" t="s">
-        <v>15</v>
+        <v>68</v>
       </c>
       <c r="H32" s="1" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="I32" s="1">
         <v>25</v>
       </c>
-    </row>
-    <row r="33" spans="6:9" x14ac:dyDescent="0.3">
+      <c r="J32" s="1">
+        <v>16</v>
+      </c>
+      <c r="K32" s="1">
+        <v>31</v>
+      </c>
+      <c r="M32" s="2" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="33" spans="6:13" x14ac:dyDescent="0.25">
       <c r="F33" s="1">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="G33" s="1" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="H33" s="1" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="I33" s="1">
         <v>18</v>
       </c>
     </row>
-    <row r="34" spans="6:9" x14ac:dyDescent="0.3">
+    <row r="34" spans="6:13" x14ac:dyDescent="0.25">
       <c r="F34" s="1">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="G34" s="1" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="H34" s="1" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="I34" s="1">
         <v>30</v>
       </c>
     </row>
-    <row r="35" spans="6:9" x14ac:dyDescent="0.3">
+    <row r="35" spans="6:13" x14ac:dyDescent="0.25">
       <c r="F35" s="1">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="G35" s="1" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="H35" s="1" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="I35" s="1">
         <v>40</v>
       </c>
     </row>
-    <row r="36" spans="6:9" x14ac:dyDescent="0.3">
+    <row r="36" spans="6:13" x14ac:dyDescent="0.25">
       <c r="F36" s="1">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="G36" s="1" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="H36" s="1" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="I36" s="1">
         <v>35</v>
       </c>
     </row>
-    <row r="37" spans="6:9" x14ac:dyDescent="0.3">
+    <row r="37" spans="6:13" x14ac:dyDescent="0.25">
       <c r="F37" s="1">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="G37" s="1" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="H37" s="1" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="I37" s="1">
         <v>15</v>
       </c>
-    </row>
-    <row r="38" spans="6:9" x14ac:dyDescent="0.3">
+      <c r="J37" s="1">
+        <v>10</v>
+      </c>
+      <c r="K37" s="1">
+        <v>25</v>
+      </c>
+      <c r="M37" s="2" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="38" spans="6:13" x14ac:dyDescent="0.25">
       <c r="F38" s="1">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="G38" s="1" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="H38" s="1" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="I38" s="1">
         <v>20</v>
       </c>
     </row>
-    <row r="39" spans="6:9" x14ac:dyDescent="0.3">
+    <row r="39" spans="6:13" x14ac:dyDescent="0.25">
       <c r="F39" s="1">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="G39" s="1" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="H39" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="I39" s="1">
+        <v>10</v>
+      </c>
+      <c r="J39" s="1">
+        <v>10</v>
+      </c>
+      <c r="K39" s="1">
+        <v>20</v>
+      </c>
+      <c r="M39" s="2" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="40" spans="6:13" x14ac:dyDescent="0.25">
+      <c r="F40" s="1">
+        <v>112</v>
+      </c>
+      <c r="G40" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="H40" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="I40" s="1">
+        <v>10</v>
+      </c>
+      <c r="J40" s="1">
+        <v>20</v>
+      </c>
+      <c r="K40" s="1">
         <v>30</v>
       </c>
-      <c r="I39" s="1">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="60" spans="4:10" x14ac:dyDescent="0.3">
+      <c r="M40" s="2" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="60" spans="4:10" x14ac:dyDescent="0.25">
       <c r="D60" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="F60" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="G60" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="F60" s="1" t="s">
+      <c r="H60" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="G60" s="1" t="s">
+      <c r="I60" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="H60" s="1" t="s">
+      <c r="J60" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="I60" s="1" t="s">
+    </row>
+    <row r="67" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C67" s="1" t="s">
         <v>41</v>
-      </c>
-      <c r="J60" s="1" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="67" spans="3:3" x14ac:dyDescent="0.3">
-      <c r="C67" s="1" t="s">
-        <v>43</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Small Tweaks / View doesn`t work yet
</commit_message>
<xml_diff>
--- a/src/main/resources/database_sample.xlsx
+++ b/src/main/resources/database_sample.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Programs\BikeRevolution\src\main\resources\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Noel\IdeaProjects\BikeRevolution\src\main\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1A4859DC-2CC7-4938-85F8-BA71004F10C1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{508D87F7-A47A-4764-A288-6E9FCD2A37B4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="22932" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{9068C110-C1AA-4A37-A3C4-5020E67D4199}"/>
+    <workbookView xWindow="22932" yWindow="1392" windowWidth="23256" windowHeight="12576" xr2:uid="{9068C110-C1AA-4A37-A3C4-5020E67D4199}"/>
   </bookViews>
   <sheets>
     <sheet name="Munka1" sheetId="1" r:id="rId1"/>
@@ -648,8 +648,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6EC0C065-1181-41F5-9F90-6272D8EE9D84}">
   <dimension ref="C1:O67"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E22" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="H30" sqref="H30"/>
+    <sheetView tabSelected="1" topLeftCell="E26" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="G25" sqref="G25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1034,7 +1034,7 @@
     </row>
     <row r="29" spans="4:15" x14ac:dyDescent="0.25">
       <c r="F29" s="1">
-        <v>101</v>
+        <v>1</v>
       </c>
       <c r="G29" s="1" t="s">
         <v>40</v>
@@ -1057,7 +1057,7 @@
     </row>
     <row r="30" spans="4:15" x14ac:dyDescent="0.25">
       <c r="F30" s="1">
-        <v>102</v>
+        <v>2</v>
       </c>
       <c r="G30" s="1" t="s">
         <v>41</v>
@@ -1080,7 +1080,7 @@
     </row>
     <row r="31" spans="4:15" x14ac:dyDescent="0.25">
       <c r="F31" s="1">
-        <v>103</v>
+        <v>3</v>
       </c>
       <c r="G31" s="1" t="s">
         <v>9</v>
@@ -1103,7 +1103,7 @@
     </row>
     <row r="32" spans="4:15" x14ac:dyDescent="0.25">
       <c r="F32" s="1">
-        <v>104</v>
+        <v>4</v>
       </c>
       <c r="G32" s="1" t="s">
         <v>72</v>
@@ -1126,7 +1126,7 @@
     </row>
     <row r="33" spans="6:13" x14ac:dyDescent="0.25">
       <c r="F33" s="1">
-        <v>105</v>
+        <v>5</v>
       </c>
       <c r="G33" s="1" t="s">
         <v>11</v>
@@ -1149,7 +1149,7 @@
     </row>
     <row r="34" spans="6:13" x14ac:dyDescent="0.25">
       <c r="F34" s="1">
-        <v>106</v>
+        <v>6</v>
       </c>
       <c r="G34" s="1" t="s">
         <v>12</v>
@@ -1166,7 +1166,7 @@
     </row>
     <row r="35" spans="6:13" x14ac:dyDescent="0.25">
       <c r="F35" s="1">
-        <v>107</v>
+        <v>7</v>
       </c>
       <c r="G35" s="1" t="s">
         <v>60</v>
@@ -1189,7 +1189,7 @@
     </row>
     <row r="36" spans="6:13" x14ac:dyDescent="0.25">
       <c r="F36" s="1">
-        <v>108</v>
+        <v>8</v>
       </c>
       <c r="G36" s="1" t="s">
         <v>14</v>
@@ -1212,7 +1212,7 @@
     </row>
     <row r="37" spans="6:13" x14ac:dyDescent="0.25">
       <c r="F37" s="1">
-        <v>109</v>
+        <v>9</v>
       </c>
       <c r="G37" s="1" t="s">
         <v>15</v>
@@ -1235,7 +1235,7 @@
     </row>
     <row r="38" spans="6:13" x14ac:dyDescent="0.25">
       <c r="F38" s="1">
-        <v>110</v>
+        <v>10</v>
       </c>
       <c r="G38" s="1" t="s">
         <v>16</v>
@@ -1258,7 +1258,7 @@
     </row>
     <row r="39" spans="6:13" x14ac:dyDescent="0.25">
       <c r="F39" s="1">
-        <v>111</v>
+        <v>11</v>
       </c>
       <c r="G39" s="1" t="s">
         <v>17</v>
@@ -1281,7 +1281,7 @@
     </row>
     <row r="40" spans="6:13" x14ac:dyDescent="0.25">
       <c r="F40" s="1">
-        <v>112</v>
+        <v>12</v>
       </c>
       <c r="G40" s="1" t="s">
         <v>48</v>

</xml_diff>

<commit_message>
New db table and some features appear in the GUI
</commit_message>
<xml_diff>
--- a/src/main/resources/database_sample.xlsx
+++ b/src/main/resources/database_sample.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Programs\BikeRevolution\src\main\resources\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Noel\IdeaProjects\BikeRevolution\src\main\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CC4F76AA-2AF6-4D85-9082-654E8D876FEB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D360C9FB-2E6E-4746-9A59-6FD867684077}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" xr2:uid="{9068C110-C1AA-4A37-A3C4-5020E67D4199}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="79">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="75">
   <si>
     <t>Description</t>
   </si>
@@ -261,18 +261,6 @@
   </si>
   <si>
     <t>[-1 váltóbowden és -1 láncolaj]</t>
-  </si>
-  <si>
-    <t>Név</t>
-  </si>
-  <si>
-    <t>Telefonszám</t>
-  </si>
-  <si>
-    <t>Időpont</t>
-  </si>
-  <si>
-    <t>Leírás</t>
   </si>
 </sst>
 </file>
@@ -645,8 +633,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6EC0C065-1181-41F5-9F90-6272D8EE9D84}">
   <dimension ref="C1:O67"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E31" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="H52" sqref="H52"/>
+    <sheetView tabSelected="1" topLeftCell="E1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="H64" sqref="H64"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1299,21 +1287,9 @@
         <v>44</v>
       </c>
     </row>
-    <row r="60" spans="4:9" x14ac:dyDescent="0.25">
+    <row r="60" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D60" s="1" t="s">
         <v>23</v>
-      </c>
-      <c r="F60" s="1" t="s">
-        <v>75</v>
-      </c>
-      <c r="G60" s="1" t="s">
-        <v>76</v>
-      </c>
-      <c r="H60" s="1" t="s">
-        <v>77</v>
-      </c>
-      <c r="I60" s="1" t="s">
-        <v>78</v>
       </c>
     </row>
     <row r="67" spans="3:3" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Add part quantity works, foglalas shows on foglalas tab
</commit_message>
<xml_diff>
--- a/src/main/resources/database_sample.xlsx
+++ b/src/main/resources/database_sample.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Noel\IdeaProjects\BikeRevolution\src\main\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D360C9FB-2E6E-4746-9A59-6FD867684077}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3FFBD10E-BEF4-4321-B665-17450F4CC112}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" xr2:uid="{9068C110-C1AA-4A37-A3C4-5020E67D4199}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="75">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83" uniqueCount="79">
   <si>
     <t>Description</t>
   </si>
@@ -251,16 +251,28 @@
     <t>Kormány és kormányszár beállítása/zsírzás</t>
   </si>
   <si>
-    <t>[-1 fékpofa -1 féktárcsa]</t>
-  </si>
-  <si>
-    <t>[-1 kormányfej -1 kenőzsír]</t>
-  </si>
-  <si>
-    <t>[-1 kenőzsír]</t>
-  </si>
-  <si>
-    <t>[-1 váltóbowden és -1 láncolaj]</t>
+    <t>PARTS</t>
+  </si>
+  <si>
+    <t>REPAIRS</t>
+  </si>
+  <si>
+    <t>REPAIRCOMPONENTS</t>
+  </si>
+  <si>
+    <t>REPAIRCOMPONENTSID</t>
+  </si>
+  <si>
+    <t>-1 váltóbowden  -1 láncolaj</t>
+  </si>
+  <si>
+    <t>-1 fékpofa -1 féktárcsa</t>
+  </si>
+  <si>
+    <t>-1 kormányfej -1 kenőzsír</t>
+  </si>
+  <si>
+    <t>-1 kenőzsír</t>
   </si>
 </sst>
 </file>
@@ -292,7 +304,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -300,12 +312,27 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -314,6 +341,9 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -634,7 +664,7 @@
   <dimension ref="C1:O67"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="E1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="H64" sqref="H64"/>
+      <selection activeCell="L6" sqref="L6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -647,8 +677,9 @@
     <col min="7" max="7" width="37.42578125" style="1" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="39.140625" style="1" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="14.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="12" style="1" bestFit="1" customWidth="1"/>
-    <col min="11" max="12" width="8.85546875" style="1"/>
+    <col min="10" max="10" width="22.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="29.7109375" style="1" customWidth="1"/>
+    <col min="12" max="12" width="28.7109375" style="1" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="24.5703125" style="1" bestFit="1" customWidth="1"/>
     <col min="14" max="16384" width="8.85546875" style="1"/>
   </cols>
@@ -661,12 +692,21 @@
         <v>29</v>
       </c>
     </row>
-    <row r="4" spans="3:15" x14ac:dyDescent="0.25">
+    <row r="2" spans="3:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="3" spans="3:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="E3" s="4" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="4" spans="3:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D4" s="1" t="s">
         <v>25</v>
       </c>
       <c r="E4" s="1" t="s">
         <v>21</v>
+      </c>
+      <c r="J4" s="4" t="s">
+        <v>73</v>
       </c>
     </row>
     <row r="5" spans="3:15" x14ac:dyDescent="0.25">
@@ -682,6 +722,9 @@
       <c r="H5" s="1" t="s">
         <v>57</v>
       </c>
+      <c r="J5" s="1" t="s">
+        <v>21</v>
+      </c>
       <c r="O5"/>
     </row>
     <row r="6" spans="3:15" x14ac:dyDescent="0.25">
@@ -697,6 +740,12 @@
       <c r="H6" s="1">
         <v>10</v>
       </c>
+      <c r="J6" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="K6" s="1" t="s">
+        <v>6</v>
+      </c>
       <c r="O6"/>
     </row>
     <row r="7" spans="3:15" x14ac:dyDescent="0.25">
@@ -712,6 +761,15 @@
       <c r="H7" s="1">
         <v>10</v>
       </c>
+      <c r="J7" s="1">
+        <v>1</v>
+      </c>
+      <c r="K7" s="1">
+        <v>1</v>
+      </c>
+      <c r="L7" s="1">
+        <v>-1</v>
+      </c>
       <c r="O7"/>
     </row>
     <row r="8" spans="3:15" x14ac:dyDescent="0.25">
@@ -727,6 +785,9 @@
       <c r="H8" s="1">
         <v>5</v>
       </c>
+      <c r="J8" s="1">
+        <v>2</v>
+      </c>
       <c r="O8"/>
     </row>
     <row r="9" spans="3:15" x14ac:dyDescent="0.25">
@@ -742,6 +803,9 @@
       <c r="H9" s="1">
         <v>15</v>
       </c>
+      <c r="J9" s="1">
+        <v>3</v>
+      </c>
       <c r="O9"/>
     </row>
     <row r="10" spans="3:15" x14ac:dyDescent="0.25">
@@ -757,6 +821,9 @@
       <c r="H10" s="1">
         <v>8</v>
       </c>
+      <c r="J10" s="1">
+        <v>4</v>
+      </c>
       <c r="O10"/>
     </row>
     <row r="11" spans="3:15" x14ac:dyDescent="0.25">
@@ -772,6 +839,9 @@
       <c r="H11" s="1">
         <v>5</v>
       </c>
+      <c r="J11" s="1">
+        <v>5</v>
+      </c>
       <c r="O11"/>
     </row>
     <row r="12" spans="3:15" x14ac:dyDescent="0.25">
@@ -787,6 +857,9 @@
       <c r="H12" s="1">
         <v>30</v>
       </c>
+      <c r="J12" s="1">
+        <v>6</v>
+      </c>
       <c r="O12"/>
     </row>
     <row r="13" spans="3:15" x14ac:dyDescent="0.25">
@@ -802,6 +875,9 @@
       <c r="H13" s="1">
         <v>20</v>
       </c>
+      <c r="J13" s="1">
+        <v>7</v>
+      </c>
       <c r="O13"/>
     </row>
     <row r="14" spans="3:15" x14ac:dyDescent="0.25">
@@ -817,6 +893,9 @@
       <c r="H14" s="1">
         <v>25</v>
       </c>
+      <c r="J14" s="1">
+        <v>8</v>
+      </c>
       <c r="O14"/>
     </row>
     <row r="15" spans="3:15" x14ac:dyDescent="0.25">
@@ -832,6 +911,9 @@
       <c r="H15" s="1">
         <v>5</v>
       </c>
+      <c r="J15" s="1">
+        <v>9</v>
+      </c>
       <c r="O15"/>
     </row>
     <row r="16" spans="3:15" x14ac:dyDescent="0.25">
@@ -847,6 +929,9 @@
       <c r="H16" s="1">
         <v>20</v>
       </c>
+      <c r="J16" s="1">
+        <v>10</v>
+      </c>
       <c r="O16"/>
     </row>
     <row r="17" spans="4:15" x14ac:dyDescent="0.25">
@@ -862,6 +947,9 @@
       <c r="H17" s="1">
         <v>15</v>
       </c>
+      <c r="J17" s="1">
+        <v>11</v>
+      </c>
       <c r="O17"/>
     </row>
     <row r="18" spans="4:15" x14ac:dyDescent="0.25">
@@ -877,6 +965,15 @@
       <c r="H18" s="1">
         <v>15</v>
       </c>
+      <c r="J18" s="1">
+        <v>12</v>
+      </c>
+      <c r="K18" s="1">
+        <v>2</v>
+      </c>
+      <c r="L18" s="1">
+        <v>-2</v>
+      </c>
       <c r="O18"/>
     </row>
     <row r="19" spans="4:15" x14ac:dyDescent="0.25">
@@ -977,313 +1074,320 @@
         <v>5</v>
       </c>
     </row>
-    <row r="27" spans="4:15" x14ac:dyDescent="0.25">
+    <row r="27" spans="4:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D27" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="F27" s="1" t="s">
+    </row>
+    <row r="28" spans="4:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="E28" s="4" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="29" spans="4:15" x14ac:dyDescent="0.25">
+      <c r="E29" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="I27" s="1" t="s">
+      <c r="H29" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="J27" s="1" t="s">
+      <c r="I29" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="M27" s="1" t="s">
+      <c r="L29" s="1" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="28" spans="4:15" x14ac:dyDescent="0.25">
-      <c r="F28" s="1" t="s">
+    <row r="30" spans="4:15" x14ac:dyDescent="0.25">
+      <c r="E30" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="G28" s="1" t="s">
+      <c r="F30" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="H28" s="1" t="s">
+      <c r="G30" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="I28" s="1" t="s">
+      <c r="H30" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="J28" s="1" t="s">
+      <c r="I30" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="K28" s="1" t="s">
+      <c r="J30" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="M28" s="1" t="s">
+      <c r="L30" s="1" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="29" spans="4:15" x14ac:dyDescent="0.25">
-      <c r="F29" s="1">
+    <row r="31" spans="4:15" x14ac:dyDescent="0.25">
+      <c r="E31" s="1">
         <v>1</v>
       </c>
-      <c r="G29" s="1" t="s">
+      <c r="F31" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="H29" s="1" t="s">
+      <c r="G31" s="1" t="s">
         <v>59</v>
       </c>
-      <c r="I29" s="1">
+      <c r="H31" s="1">
         <v>15</v>
       </c>
-      <c r="J29" s="1">
+      <c r="I31" s="1">
         <v>18</v>
       </c>
-      <c r="K29" s="1">
+      <c r="J31" s="1">
         <v>33</v>
       </c>
-      <c r="M29" s="2" t="s">
+      <c r="L31" s="2" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="30" spans="4:15" x14ac:dyDescent="0.25">
-      <c r="F30" s="1">
+    <row r="32" spans="4:15" x14ac:dyDescent="0.25">
+      <c r="E32" s="1">
         <v>2</v>
       </c>
-      <c r="G30" s="1" t="s">
+      <c r="F32" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="H30" s="1" t="s">
+      <c r="G32" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="I30" s="1">
+      <c r="H32" s="1">
         <v>10</v>
       </c>
-      <c r="J30" s="1">
+      <c r="I32" s="1">
         <v>5</v>
       </c>
-      <c r="K30" s="1">
+      <c r="J32" s="1">
         <v>15</v>
       </c>
-      <c r="M30" s="2" t="s">
+      <c r="L32" s="2" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="31" spans="4:15" x14ac:dyDescent="0.25">
-      <c r="F31" s="1">
+    <row r="33" spans="5:12" x14ac:dyDescent="0.25">
+      <c r="E33" s="1">
         <v>3</v>
       </c>
-      <c r="G31" s="1" t="s">
+      <c r="F33" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="H31" s="1" t="s">
+      <c r="G33" s="1" t="s">
         <v>60</v>
       </c>
-      <c r="I31" s="1">
+      <c r="H33" s="1">
         <v>20</v>
       </c>
-      <c r="J31" s="1">
+      <c r="I33" s="1">
         <v>20</v>
       </c>
-      <c r="K31" s="1">
+      <c r="J33" s="1">
         <v>40</v>
       </c>
-      <c r="M31" s="2" t="s">
+      <c r="L33" s="2" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="32" spans="4:15" x14ac:dyDescent="0.25">
-      <c r="F32" s="1">
+    <row r="34" spans="5:12" x14ac:dyDescent="0.25">
+      <c r="E34" s="1">
         <v>4</v>
       </c>
-      <c r="G32" s="1" t="s">
+      <c r="F34" s="1" t="s">
         <v>67</v>
       </c>
-      <c r="H32" s="1" t="s">
+      <c r="G34" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="I32" s="1">
+      <c r="H34" s="1">
         <v>25</v>
       </c>
-      <c r="J32" s="1">
+      <c r="I34" s="1">
         <v>13</v>
       </c>
-      <c r="K32" s="1">
+      <c r="J34" s="1">
         <v>38</v>
       </c>
-      <c r="M32" s="2" t="s">
+      <c r="L34" s="2" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="33" spans="6:13" x14ac:dyDescent="0.25">
-      <c r="F33" s="1">
+    <row r="35" spans="5:12" x14ac:dyDescent="0.25">
+      <c r="E35" s="1">
         <v>5</v>
       </c>
-      <c r="G33" s="1" t="s">
+      <c r="F35" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="H33" s="1" t="s">
+      <c r="G35" s="1" t="s">
         <v>68</v>
       </c>
-      <c r="I33" s="1">
+      <c r="H35" s="1">
         <v>18</v>
       </c>
-      <c r="J33" s="1">
+      <c r="I35" s="1">
         <v>10</v>
       </c>
-      <c r="K33" s="1">
+      <c r="J35" s="1">
         <v>28</v>
       </c>
-      <c r="M33" s="1" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="34" spans="6:13" x14ac:dyDescent="0.25">
-      <c r="F34" s="1">
+      <c r="L35" s="2" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="36" spans="5:12" x14ac:dyDescent="0.25">
+      <c r="E36" s="1">
         <v>6</v>
       </c>
-      <c r="G34" s="1" t="s">
+      <c r="F36" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="H34" s="1" t="s">
+      <c r="G36" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="I34" s="1">
+      <c r="H36" s="1">
         <v>30</v>
-      </c>
-      <c r="K34" s="1">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="35" spans="6:13" x14ac:dyDescent="0.25">
-      <c r="F35" s="1">
-        <v>7</v>
-      </c>
-      <c r="G35" s="1" t="s">
-        <v>55</v>
-      </c>
-      <c r="H35" s="1" t="s">
-        <v>61</v>
-      </c>
-      <c r="I35" s="1">
-        <v>40</v>
-      </c>
-      <c r="J35" s="1">
-        <v>38</v>
-      </c>
-      <c r="K35" s="1">
-        <v>78</v>
-      </c>
-      <c r="M35" s="1" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="36" spans="6:13" x14ac:dyDescent="0.25">
-      <c r="F36" s="1">
-        <v>8</v>
-      </c>
-      <c r="G36" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="H36" s="1" t="s">
-        <v>62</v>
-      </c>
-      <c r="I36" s="1">
-        <v>35</v>
       </c>
       <c r="J36" s="1">
         <v>30</v>
       </c>
-      <c r="K36" s="1">
+    </row>
+    <row r="37" spans="5:12" x14ac:dyDescent="0.25">
+      <c r="E37" s="1">
+        <v>7</v>
+      </c>
+      <c r="F37" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="G37" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="H37" s="1">
+        <v>40</v>
+      </c>
+      <c r="I37" s="1">
+        <v>38</v>
+      </c>
+      <c r="J37" s="1">
+        <v>78</v>
+      </c>
+      <c r="L37" s="2" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="38" spans="5:12" x14ac:dyDescent="0.25">
+      <c r="E38" s="1">
+        <v>8</v>
+      </c>
+      <c r="F38" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="G38" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="H38" s="1">
+        <v>35</v>
+      </c>
+      <c r="I38" s="1">
+        <v>30</v>
+      </c>
+      <c r="J38" s="1">
         <v>65</v>
       </c>
-      <c r="M36" s="1" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="37" spans="6:13" x14ac:dyDescent="0.25">
-      <c r="F37" s="1">
+      <c r="L38" s="2" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="39" spans="5:12" x14ac:dyDescent="0.25">
+      <c r="E39" s="1">
         <v>9</v>
       </c>
-      <c r="G37" s="1" t="s">
+      <c r="F39" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="H37" s="1" t="s">
+      <c r="G39" s="1" t="s">
         <v>63</v>
       </c>
-      <c r="I37" s="1">
+      <c r="H39" s="1">
         <v>15</v>
       </c>
-      <c r="J37" s="1">
+      <c r="I39" s="1">
         <v>15</v>
       </c>
-      <c r="K37" s="1">
+      <c r="J39" s="1">
         <v>30</v>
       </c>
-      <c r="M37" s="2" t="s">
+      <c r="L39" s="2" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="38" spans="6:13" x14ac:dyDescent="0.25">
-      <c r="F38" s="1">
+    <row r="40" spans="5:12" x14ac:dyDescent="0.25">
+      <c r="E40" s="1">
         <v>10</v>
       </c>
-      <c r="G38" s="1" t="s">
+      <c r="F40" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="H38" s="1" t="s">
+      <c r="G40" s="1" t="s">
         <v>70</v>
       </c>
-      <c r="I38" s="1">
+      <c r="H40" s="1">
         <v>20</v>
       </c>
-      <c r="J38" s="1">
+      <c r="I40" s="1">
         <v>5</v>
       </c>
-      <c r="K38" s="1">
+      <c r="J40" s="1">
         <v>25</v>
       </c>
-      <c r="M38" s="1" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="39" spans="6:13" x14ac:dyDescent="0.25">
-      <c r="F39" s="1">
+      <c r="L40" s="2" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="41" spans="5:12" x14ac:dyDescent="0.25">
+      <c r="E41" s="1">
         <v>11</v>
       </c>
-      <c r="G39" s="1" t="s">
+      <c r="F41" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="H39" s="1" t="s">
+      <c r="G41" s="1" t="s">
         <v>64</v>
       </c>
-      <c r="I39" s="1">
+      <c r="H41" s="1">
         <v>10</v>
       </c>
-      <c r="J39" s="1">
+      <c r="I41" s="1">
         <v>15</v>
       </c>
-      <c r="K39" s="1">
+      <c r="J41" s="1">
         <v>25</v>
       </c>
-      <c r="M39" s="2" t="s">
+      <c r="L41" s="2" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="40" spans="6:13" x14ac:dyDescent="0.25">
-      <c r="F40" s="1">
+    <row r="42" spans="5:12" x14ac:dyDescent="0.25">
+      <c r="E42" s="1">
         <v>12</v>
       </c>
-      <c r="G40" s="1" t="s">
+      <c r="F42" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="H40" s="1" t="s">
+      <c r="G42" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="I40" s="1">
+      <c r="H42" s="1">
         <v>10</v>
       </c>
-      <c r="J40" s="1">
+      <c r="I42" s="1">
         <v>20</v>
       </c>
-      <c r="K40" s="1">
+      <c r="J42" s="1">
         <v>30</v>
       </c>
-      <c r="M40" s="2" t="s">
+      <c r="L42" s="2" t="s">
         <v>44</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Reservation m-f, new table ResourceCost
</commit_message>
<xml_diff>
--- a/src/main/resources/database_sample.xlsx
+++ b/src/main/resources/database_sample.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Noel\IdeaProjects\BikeRevolution\src\main\resources\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Programs\BikeRevolution\src\main\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3FFBD10E-BEF4-4321-B665-17450F4CC112}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{72634701-B7EE-4953-A625-9212D38B3893}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" xr2:uid="{9068C110-C1AA-4A37-A3C4-5020E67D4199}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83" uniqueCount="79">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="103" uniqueCount="91">
   <si>
     <t>Description</t>
   </si>
@@ -107,12 +107,6 @@
     <t>LABORCOST(eur)</t>
   </si>
   <si>
-    <t>Foglalás Tábla</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Webes Loginhoz Tábla</t>
-  </si>
-  <si>
     <t>PARTS TABLE</t>
   </si>
   <si>
@@ -185,9 +179,6 @@
     <t>Ez sem kell a táblába</t>
   </si>
   <si>
-    <t>-2 fekbetet</t>
-  </si>
-  <si>
     <t>Váltó</t>
   </si>
   <si>
@@ -273,6 +264,51 @@
   </si>
   <si>
     <t>-1 kenőzsír</t>
+  </si>
+  <si>
+    <t>-2 fekpofa</t>
+  </si>
+  <si>
+    <t>RESOURCECOST</t>
+  </si>
+  <si>
+    <t>RESOURCECOST TÁBLA</t>
+  </si>
+  <si>
+    <t>PARD_ID</t>
+  </si>
+  <si>
+    <t>1 19</t>
+  </si>
+  <si>
+    <t>PART_QUANTITY</t>
+  </si>
+  <si>
+    <t>4 17</t>
+  </si>
+  <si>
+    <t>5 15</t>
+  </si>
+  <si>
+    <t>17 20</t>
+  </si>
+  <si>
+    <t>5 7</t>
+  </si>
+  <si>
+    <t>-1 -1</t>
+  </si>
+  <si>
+    <t>9 18</t>
+  </si>
+  <si>
+    <t>10 18</t>
+  </si>
+  <si>
+    <t>-2 -1</t>
+  </si>
+  <si>
+    <t>14 18</t>
   </si>
 </sst>
 </file>
@@ -661,10 +697,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6EC0C065-1181-41F5-9F90-6272D8EE9D84}">
-  <dimension ref="C1:O67"/>
+  <dimension ref="C1:O59"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="L6" sqref="L6"/>
+    <sheetView tabSelected="1" topLeftCell="D22" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="J33" sqref="J33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -672,8 +708,8 @@
     <col min="1" max="2" width="8.85546875" style="1"/>
     <col min="3" max="3" width="21.28515625" style="1" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="34.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="11.28515625" style="1" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="30" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="14.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="36.5703125" style="1" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="37.42578125" style="1" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="39.140625" style="1" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="14.7109375" style="1" bestFit="1" customWidth="1"/>
@@ -686,27 +722,27 @@
   <sheetData>
     <row r="1" spans="3:15" x14ac:dyDescent="0.25">
       <c r="C1" s="1" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="D1" s="3" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
     </row>
     <row r="2" spans="3:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="3" spans="3:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="E3" s="4" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
     </row>
     <row r="4" spans="3:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D4" s="1" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="E4" s="1" t="s">
         <v>21</v>
       </c>
       <c r="J4" s="4" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
     </row>
     <row r="5" spans="3:15" x14ac:dyDescent="0.25">
@@ -720,7 +756,7 @@
         <v>8</v>
       </c>
       <c r="H5" s="1" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="J5" s="1" t="s">
         <v>21</v>
@@ -741,7 +777,7 @@
         <v>10</v>
       </c>
       <c r="J6" s="1" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="K6" s="1" t="s">
         <v>6</v>
@@ -753,7 +789,7 @@
         <v>2</v>
       </c>
       <c r="F7" s="1" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="G7" s="1">
         <v>50</v>
@@ -777,7 +813,7 @@
         <v>3</v>
       </c>
       <c r="F8" s="1" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="G8" s="1">
         <v>30</v>
@@ -813,7 +849,7 @@
         <v>5</v>
       </c>
       <c r="F10" s="1" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="G10" s="1">
         <v>40</v>
@@ -831,7 +867,7 @@
         <v>6</v>
       </c>
       <c r="F11" s="1" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="G11" s="1">
         <v>50</v>
@@ -849,7 +885,7 @@
         <v>7</v>
       </c>
       <c r="F12" s="1" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="G12" s="1">
         <v>25</v>
@@ -867,7 +903,7 @@
         <v>8</v>
       </c>
       <c r="F13" s="1" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="G13" s="1">
         <v>20</v>
@@ -921,7 +957,7 @@
         <v>11</v>
       </c>
       <c r="F16" s="1" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="G16" s="1">
         <v>20</v>
@@ -939,7 +975,7 @@
         <v>12</v>
       </c>
       <c r="F17" s="1" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="G17" s="1">
         <v>20</v>
@@ -957,7 +993,7 @@
         <v>13</v>
       </c>
       <c r="F18" s="1" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="G18" s="1">
         <v>20</v>
@@ -995,7 +1031,7 @@
         <v>15</v>
       </c>
       <c r="F20" s="1" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="G20" s="1">
         <v>30</v>
@@ -1009,7 +1045,7 @@
         <v>16</v>
       </c>
       <c r="F21" s="1" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="G21" s="1">
         <v>40</v>
@@ -1023,7 +1059,7 @@
         <v>17</v>
       </c>
       <c r="F22" s="1" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="G22" s="1">
         <v>20</v>
@@ -1037,7 +1073,7 @@
         <v>18</v>
       </c>
       <c r="F23" s="1" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="G23" s="1">
         <v>10</v>
@@ -1051,7 +1087,7 @@
         <v>19</v>
       </c>
       <c r="F24" s="1" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="G24" s="1">
         <v>15</v>
@@ -1065,7 +1101,7 @@
         <v>20</v>
       </c>
       <c r="F25" s="1" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="G25" s="1">
         <v>25</v>
@@ -1081,7 +1117,7 @@
     </row>
     <row r="28" spans="4:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="E28" s="4" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
     </row>
     <row r="29" spans="4:15" x14ac:dyDescent="0.25">
@@ -1089,13 +1125,13 @@
         <v>21</v>
       </c>
       <c r="H29" s="1" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="I29" s="1" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="L29" s="1" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
     </row>
     <row r="30" spans="4:15" x14ac:dyDescent="0.25">
@@ -1112,13 +1148,13 @@
         <v>22</v>
       </c>
       <c r="I30" s="1" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="J30" s="1" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="L30" s="1" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
     </row>
     <row r="31" spans="4:15" x14ac:dyDescent="0.25">
@@ -1126,10 +1162,10 @@
         <v>1</v>
       </c>
       <c r="F31" s="1" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="G31" s="1" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="H31" s="1">
         <v>15</v>
@@ -1141,7 +1177,7 @@
         <v>33</v>
       </c>
       <c r="L31" s="2" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
     </row>
     <row r="32" spans="4:15" x14ac:dyDescent="0.25">
@@ -1149,10 +1185,10 @@
         <v>2</v>
       </c>
       <c r="F32" s="1" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="G32" s="1" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="H32" s="1">
         <v>10</v>
@@ -1164,10 +1200,10 @@
         <v>15</v>
       </c>
       <c r="L32" s="2" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="33" spans="5:12" x14ac:dyDescent="0.25">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="33" spans="4:12" x14ac:dyDescent="0.25">
       <c r="E33" s="1">
         <v>3</v>
       </c>
@@ -1175,7 +1211,7 @@
         <v>9</v>
       </c>
       <c r="G33" s="1" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="H33" s="1">
         <v>20</v>
@@ -1187,15 +1223,15 @@
         <v>40</v>
       </c>
       <c r="L33" s="2" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="34" spans="5:12" x14ac:dyDescent="0.25">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="34" spans="4:12" x14ac:dyDescent="0.25">
       <c r="E34" s="1">
         <v>4</v>
       </c>
       <c r="F34" s="1" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="G34" s="1" t="s">
         <v>10</v>
@@ -1210,10 +1246,10 @@
         <v>38</v>
       </c>
       <c r="L34" s="2" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="35" spans="5:12" x14ac:dyDescent="0.25">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="35" spans="4:12" x14ac:dyDescent="0.25">
       <c r="E35" s="1">
         <v>5</v>
       </c>
@@ -1221,7 +1257,7 @@
         <v>11</v>
       </c>
       <c r="G35" s="1" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="H35" s="1">
         <v>18</v>
@@ -1233,10 +1269,10 @@
         <v>28</v>
       </c>
       <c r="L35" s="2" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="36" spans="5:12" x14ac:dyDescent="0.25">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="36" spans="4:12" x14ac:dyDescent="0.25">
       <c r="E36" s="1">
         <v>6</v>
       </c>
@@ -1253,15 +1289,15 @@
         <v>30</v>
       </c>
     </row>
-    <row r="37" spans="5:12" x14ac:dyDescent="0.25">
+    <row r="37" spans="4:12" x14ac:dyDescent="0.25">
       <c r="E37" s="1">
         <v>7</v>
       </c>
       <c r="F37" s="1" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="G37" s="1" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="H37" s="1">
         <v>40</v>
@@ -1273,10 +1309,10 @@
         <v>78</v>
       </c>
       <c r="L37" s="2" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="38" spans="5:12" x14ac:dyDescent="0.25">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="38" spans="4:12" x14ac:dyDescent="0.25">
       <c r="E38" s="1">
         <v>8</v>
       </c>
@@ -1284,7 +1320,7 @@
         <v>14</v>
       </c>
       <c r="G38" s="1" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="H38" s="1">
         <v>35</v>
@@ -1296,10 +1332,10 @@
         <v>65</v>
       </c>
       <c r="L38" s="2" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="39" spans="5:12" x14ac:dyDescent="0.25">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="39" spans="4:12" x14ac:dyDescent="0.25">
       <c r="E39" s="1">
         <v>9</v>
       </c>
@@ -1307,7 +1343,7 @@
         <v>15</v>
       </c>
       <c r="G39" s="1" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="H39" s="1">
         <v>15</v>
@@ -1319,10 +1355,10 @@
         <v>30</v>
       </c>
       <c r="L39" s="2" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="40" spans="5:12" x14ac:dyDescent="0.25">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="40" spans="4:12" x14ac:dyDescent="0.25">
       <c r="E40" s="1">
         <v>10</v>
       </c>
@@ -1330,7 +1366,7 @@
         <v>16</v>
       </c>
       <c r="G40" s="1" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="H40" s="1">
         <v>20</v>
@@ -1342,10 +1378,10 @@
         <v>25</v>
       </c>
       <c r="L40" s="2" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="41" spans="5:12" x14ac:dyDescent="0.25">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="41" spans="4:12" x14ac:dyDescent="0.25">
       <c r="E41" s="1">
         <v>11</v>
       </c>
@@ -1353,7 +1389,7 @@
         <v>17</v>
       </c>
       <c r="G41" s="1" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="H41" s="1">
         <v>10</v>
@@ -1365,18 +1401,18 @@
         <v>25</v>
       </c>
       <c r="L41" s="2" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="42" spans="5:12" x14ac:dyDescent="0.25">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="42" spans="4:12" x14ac:dyDescent="0.25">
       <c r="E42" s="1">
         <v>12</v>
       </c>
       <c r="F42" s="1" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="G42" s="1" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="H42" s="1">
         <v>10</v>
@@ -1388,17 +1424,163 @@
         <v>30</v>
       </c>
       <c r="L42" s="2" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="60" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D60" s="1" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="67" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C67" s="1" t="s">
-        <v>24</v>
+        <v>42</v>
+      </c>
+    </row>
+    <row r="45" spans="4:12" x14ac:dyDescent="0.25">
+      <c r="D45" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="E45" s="1" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="46" spans="4:12" x14ac:dyDescent="0.25">
+      <c r="E46" s="1" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="47" spans="4:12" x14ac:dyDescent="0.25">
+      <c r="E47" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="F47" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="G47" s="1" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="48" spans="4:12" x14ac:dyDescent="0.25">
+      <c r="E48" s="1">
+        <v>1</v>
+      </c>
+      <c r="F48" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="G48" s="2" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="49" spans="5:7" x14ac:dyDescent="0.25">
+      <c r="E49" s="1">
+        <v>2</v>
+      </c>
+      <c r="F49" s="1">
+        <v>3</v>
+      </c>
+      <c r="G49" s="1">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="50" spans="5:7" x14ac:dyDescent="0.25">
+      <c r="E50" s="1">
+        <v>3</v>
+      </c>
+      <c r="F50" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="G50" s="2" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="51" spans="5:7" x14ac:dyDescent="0.25">
+      <c r="E51" s="1">
+        <v>4</v>
+      </c>
+      <c r="F51" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="G51" s="2" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="52" spans="5:7" x14ac:dyDescent="0.25">
+      <c r="E52" s="1">
+        <v>5</v>
+      </c>
+      <c r="F52" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="G52" s="2" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="53" spans="5:7" x14ac:dyDescent="0.25">
+      <c r="E53" s="1">
+        <v>6</v>
+      </c>
+      <c r="F53" s="1">
+        <v>0</v>
+      </c>
+      <c r="G53" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="54" spans="5:7" x14ac:dyDescent="0.25">
+      <c r="E54" s="1">
+        <v>7</v>
+      </c>
+      <c r="F54" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="G54" s="2" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="55" spans="5:7" x14ac:dyDescent="0.25">
+      <c r="E55" s="1">
+        <v>8</v>
+      </c>
+      <c r="F55" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="G55" s="2" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="56" spans="5:7" x14ac:dyDescent="0.25">
+      <c r="E56" s="1">
+        <v>9</v>
+      </c>
+      <c r="F56" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="G56" s="2" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="57" spans="5:7" x14ac:dyDescent="0.25">
+      <c r="E57" s="1">
+        <v>10</v>
+      </c>
+      <c r="F57" s="1">
+        <v>18</v>
+      </c>
+      <c r="G57" s="1">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="58" spans="5:7" x14ac:dyDescent="0.25">
+      <c r="E58" s="1">
+        <v>11</v>
+      </c>
+      <c r="F58" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="G58" s="2" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="59" spans="5:7" x14ac:dyDescent="0.25">
+      <c r="E59" s="1">
+        <v>12</v>
+      </c>
+      <c r="F59" s="1">
+        <v>2</v>
+      </c>
+      <c r="G59" s="1">
+        <v>-2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
small decoration in excel
</commit_message>
<xml_diff>
--- a/src/main/resources/database_sample.xlsx
+++ b/src/main/resources/database_sample.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Programs\BikeRevolution\src\main\resources\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Noel\IdeaProjects\BikeRevolution\src\main\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{72634701-B7EE-4953-A625-9212D38B3893}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AE0D002C-45AD-4C9A-AF79-2F13868D0C00}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" xr2:uid="{9068C110-C1AA-4A37-A3C4-5020E67D4199}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="103" uniqueCount="91">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="99" uniqueCount="89">
   <si>
     <t>Description</t>
   </si>
@@ -246,12 +246,6 @@
   </si>
   <si>
     <t>REPAIRS</t>
-  </si>
-  <si>
-    <t>REPAIRCOMPONENTS</t>
-  </si>
-  <si>
-    <t>REPAIRCOMPONENTSID</t>
   </si>
   <si>
     <t>-1 váltóbowden  -1 láncolaj</t>
@@ -368,7 +362,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -380,6 +374,9 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -699,8 +696,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6EC0C065-1181-41F5-9F90-6272D8EE9D84}">
   <dimension ref="C1:O59"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D22" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="J33" sqref="J33"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="F23" sqref="F23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -734,16 +731,14 @@
         <v>68</v>
       </c>
     </row>
-    <row r="4" spans="3:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="3:15" x14ac:dyDescent="0.25">
       <c r="D4" s="1" t="s">
         <v>23</v>
       </c>
       <c r="E4" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="J4" s="4" t="s">
-        <v>70</v>
-      </c>
+      <c r="J4" s="5"/>
     </row>
     <row r="5" spans="3:15" x14ac:dyDescent="0.25">
       <c r="E5" s="1" t="s">
@@ -758,9 +753,6 @@
       <c r="H5" s="1" t="s">
         <v>54</v>
       </c>
-      <c r="J5" s="1" t="s">
-        <v>21</v>
-      </c>
       <c r="O5"/>
     </row>
     <row r="6" spans="3:15" x14ac:dyDescent="0.25">
@@ -776,12 +768,6 @@
       <c r="H6" s="1">
         <v>10</v>
       </c>
-      <c r="J6" s="1" t="s">
-        <v>71</v>
-      </c>
-      <c r="K6" s="1" t="s">
-        <v>6</v>
-      </c>
       <c r="O6"/>
     </row>
     <row r="7" spans="3:15" x14ac:dyDescent="0.25">
@@ -797,15 +783,6 @@
       <c r="H7" s="1">
         <v>10</v>
       </c>
-      <c r="J7" s="1">
-        <v>1</v>
-      </c>
-      <c r="K7" s="1">
-        <v>1</v>
-      </c>
-      <c r="L7" s="1">
-        <v>-1</v>
-      </c>
       <c r="O7"/>
     </row>
     <row r="8" spans="3:15" x14ac:dyDescent="0.25">
@@ -821,9 +798,6 @@
       <c r="H8" s="1">
         <v>5</v>
       </c>
-      <c r="J8" s="1">
-        <v>2</v>
-      </c>
       <c r="O8"/>
     </row>
     <row r="9" spans="3:15" x14ac:dyDescent="0.25">
@@ -839,9 +813,6 @@
       <c r="H9" s="1">
         <v>15</v>
       </c>
-      <c r="J9" s="1">
-        <v>3</v>
-      </c>
       <c r="O9"/>
     </row>
     <row r="10" spans="3:15" x14ac:dyDescent="0.25">
@@ -857,9 +828,6 @@
       <c r="H10" s="1">
         <v>8</v>
       </c>
-      <c r="J10" s="1">
-        <v>4</v>
-      </c>
       <c r="O10"/>
     </row>
     <row r="11" spans="3:15" x14ac:dyDescent="0.25">
@@ -875,9 +843,6 @@
       <c r="H11" s="1">
         <v>5</v>
       </c>
-      <c r="J11" s="1">
-        <v>5</v>
-      </c>
       <c r="O11"/>
     </row>
     <row r="12" spans="3:15" x14ac:dyDescent="0.25">
@@ -893,9 +858,6 @@
       <c r="H12" s="1">
         <v>30</v>
       </c>
-      <c r="J12" s="1">
-        <v>6</v>
-      </c>
       <c r="O12"/>
     </row>
     <row r="13" spans="3:15" x14ac:dyDescent="0.25">
@@ -911,9 +873,6 @@
       <c r="H13" s="1">
         <v>20</v>
       </c>
-      <c r="J13" s="1">
-        <v>7</v>
-      </c>
       <c r="O13"/>
     </row>
     <row r="14" spans="3:15" x14ac:dyDescent="0.25">
@@ -929,9 +888,6 @@
       <c r="H14" s="1">
         <v>25</v>
       </c>
-      <c r="J14" s="1">
-        <v>8</v>
-      </c>
       <c r="O14"/>
     </row>
     <row r="15" spans="3:15" x14ac:dyDescent="0.25">
@@ -947,9 +903,6 @@
       <c r="H15" s="1">
         <v>5</v>
       </c>
-      <c r="J15" s="1">
-        <v>9</v>
-      </c>
       <c r="O15"/>
     </row>
     <row r="16" spans="3:15" x14ac:dyDescent="0.25">
@@ -965,9 +918,6 @@
       <c r="H16" s="1">
         <v>20</v>
       </c>
-      <c r="J16" s="1">
-        <v>10</v>
-      </c>
       <c r="O16"/>
     </row>
     <row r="17" spans="4:15" x14ac:dyDescent="0.25">
@@ -983,9 +933,6 @@
       <c r="H17" s="1">
         <v>15</v>
       </c>
-      <c r="J17" s="1">
-        <v>11</v>
-      </c>
       <c r="O17"/>
     </row>
     <row r="18" spans="4:15" x14ac:dyDescent="0.25">
@@ -1001,15 +948,6 @@
       <c r="H18" s="1">
         <v>15</v>
       </c>
-      <c r="J18" s="1">
-        <v>12</v>
-      </c>
-      <c r="K18" s="1">
-        <v>2</v>
-      </c>
-      <c r="L18" s="1">
-        <v>-2</v>
-      </c>
       <c r="O18"/>
     </row>
     <row r="19" spans="4:15" x14ac:dyDescent="0.25">
@@ -1246,7 +1184,7 @@
         <v>38</v>
       </c>
       <c r="L34" s="2" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
     </row>
     <row r="35" spans="4:12" x14ac:dyDescent="0.25">
@@ -1269,7 +1207,7 @@
         <v>28</v>
       </c>
       <c r="L35" s="2" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
     </row>
     <row r="36" spans="4:12" x14ac:dyDescent="0.25">
@@ -1309,7 +1247,7 @@
         <v>78</v>
       </c>
       <c r="L37" s="2" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
     </row>
     <row r="38" spans="4:12" x14ac:dyDescent="0.25">
@@ -1332,7 +1270,7 @@
         <v>65</v>
       </c>
       <c r="L38" s="2" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
     </row>
     <row r="39" spans="4:12" x14ac:dyDescent="0.25">
@@ -1378,7 +1316,7 @@
         <v>25</v>
       </c>
       <c r="L40" s="2" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
     </row>
     <row r="41" spans="4:12" x14ac:dyDescent="0.25">
@@ -1427,12 +1365,13 @@
         <v>42</v>
       </c>
     </row>
-    <row r="45" spans="4:12" x14ac:dyDescent="0.25">
+    <row r="44" spans="4:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="45" spans="4:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D45" s="1" t="s">
-        <v>78</v>
-      </c>
-      <c r="E45" s="1" t="s">
-        <v>77</v>
+        <v>76</v>
+      </c>
+      <c r="E45" s="4" t="s">
+        <v>75</v>
       </c>
     </row>
     <row r="46" spans="4:12" x14ac:dyDescent="0.25">
@@ -1445,10 +1384,10 @@
         <v>18</v>
       </c>
       <c r="F47" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="G47" s="1" t="s">
         <v>79</v>
-      </c>
-      <c r="G47" s="1" t="s">
-        <v>81</v>
       </c>
     </row>
     <row r="48" spans="4:12" x14ac:dyDescent="0.25">
@@ -1456,10 +1395,10 @@
         <v>1</v>
       </c>
       <c r="F48" s="1" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="G48" s="2" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
     </row>
     <row r="49" spans="5:7" x14ac:dyDescent="0.25">
@@ -1478,10 +1417,10 @@
         <v>3</v>
       </c>
       <c r="F50" s="1" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="G50" s="2" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
     </row>
     <row r="51" spans="5:7" x14ac:dyDescent="0.25">
@@ -1489,10 +1428,10 @@
         <v>4</v>
       </c>
       <c r="F51" s="1" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="G51" s="2" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
     </row>
     <row r="52" spans="5:7" x14ac:dyDescent="0.25">
@@ -1500,10 +1439,10 @@
         <v>5</v>
       </c>
       <c r="F52" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="G52" s="2" t="s">
         <v>84</v>
-      </c>
-      <c r="G52" s="2" t="s">
-        <v>86</v>
       </c>
     </row>
     <row r="53" spans="5:7" x14ac:dyDescent="0.25">
@@ -1522,10 +1461,10 @@
         <v>7</v>
       </c>
       <c r="F54" s="1" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="G54" s="2" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
     </row>
     <row r="55" spans="5:7" x14ac:dyDescent="0.25">
@@ -1533,10 +1472,10 @@
         <v>8</v>
       </c>
       <c r="F55" s="1" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="G55" s="2" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
     </row>
     <row r="56" spans="5:7" x14ac:dyDescent="0.25">
@@ -1544,10 +1483,10 @@
         <v>9</v>
       </c>
       <c r="F56" s="1" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="G56" s="2" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
     </row>
     <row r="57" spans="5:7" x14ac:dyDescent="0.25">
@@ -1566,10 +1505,10 @@
         <v>11</v>
       </c>
       <c r="F58" s="1" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="G58" s="2" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
     </row>
     <row r="59" spans="5:7" x14ac:dyDescent="0.25">

</xml_diff>